<commit_message>
FHIR Dataset and store
</commit_message>
<xml_diff>
--- a/src/test/resources/Endpoint/FHIRExcel.xlsx
+++ b/src/test/resources/Endpoint/FHIRExcel.xlsx
@@ -3,31 +3,52 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4851919F-6C5A-41DB-8E67-501C3862ADE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6306726-6972-4D1B-81FD-3A1CFE0B816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Endpoint" sheetId="2" r:id="rId1"/>
+    <sheet name="CreateStoreEndpoint" sheetId="2" r:id="rId1"/>
+    <sheet name="CreateDataSetEndpoint" sheetId="3" r:id="rId2"/>
+    <sheet name="GetAllFHIRStoresEndpoint" sheetId="4" r:id="rId3"/>
+    <sheet name="UpdateTimeZoneEndpoint" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>FHIREndpoint</t>
-  </si>
-  <si>
-    <t>/projects/healthcare-system-api/locations/us-central1/datasets/healthcare_data/fhirStores?fhirStoreId=Raja_85</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>FHIRStoreEndpoint</t>
+  </si>
+  <si>
+    <t>FHIRDataSetEndpoint</t>
+  </si>
+  <si>
+    <t>/projects/healthcare-system-api/locations/us-central1/datasets?datasetId=healthcare_data</t>
+  </si>
+  <si>
+    <t>/projects/healthcare-system-api/locations/us-central1/datasets/healthcare_data/fhirStores?fhirStoreId=Dar_83</t>
+  </si>
+  <si>
+    <t>FHIRStoresEndpoint</t>
+  </si>
+  <si>
+    <t>/projects/healthcare-system-api/locations/us-central1/datasets/healthcare_data/fhirStores</t>
+  </si>
+  <si>
+    <t>FHIRUpdateDatasetEndpoint</t>
+  </si>
+  <si>
+    <t>/projects/healthcare-system-api/locations/us-central1/datasets/healthcare_data?updateMask=timeZone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +86,31 @@
       <color rgb="FF008000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -99,6 +145,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,20 +474,20 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -447,8 +498,90 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8ADCC9-F4B0-48CC-9681-B333AAFAACB3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="119.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://healthcare.googleapis.com/v1/projects/healthcare-system-api/locations/us-central1/datasets?datasetId=healthcare_data" xr:uid="{EEB58D9E-FDDB-46A9-BB75-A0712C90144F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FECCF1-1574-43AC-BD96-1A7DA552E090}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="101" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDF0512-1F01-4FE0-8121-9915F280EAC6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="145" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>